<commit_message>
Added new model classes for the tables
</commit_message>
<xml_diff>
--- a/docs/JB.xlsx
+++ b/docs/JB.xlsx
@@ -355,9 +355,6 @@
     <t>Employer pages : dynamic pages based on templates (Profile, Trainings, Success Stories)</t>
   </si>
   <si>
-    <t>As an Employer I am able to maintain the view count while viewing the resumes(Job Id)</t>
-  </si>
-  <si>
     <t>As a Employer I am able to change password</t>
   </si>
   <si>
@@ -443,6 +440,9 @@
   </si>
   <si>
     <t>/api/message/view/employer</t>
+  </si>
+  <si>
+    <t>As an Employer I am able to maintain the view count while viewing the resumes(resumeId)</t>
   </si>
 </sst>
 </file>
@@ -808,7 +808,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -854,7 +854,7 @@
         <v>59</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -865,7 +865,7 @@
         <v>60</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -876,7 +876,7 @@
         <v>61</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -887,7 +887,7 @@
         <v>62</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -898,7 +898,7 @@
         <v>63</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -909,7 +909,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -920,7 +920,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -964,7 +964,7 @@
         <v>69</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -975,7 +975,7 @@
         <v>70</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -997,7 +997,7 @@
         <v>72</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1008,7 +1008,7 @@
         <v>73</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1019,7 +1019,7 @@
         <v>74</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1030,7 +1030,7 @@
         <v>75</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1041,7 +1041,7 @@
         <v>76</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1049,10 +1049,10 @@
         <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1063,7 +1063,7 @@
         <v>77</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1074,7 +1074,7 @@
         <v>78</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1085,7 +1085,7 @@
         <v>79</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1096,7 +1096,7 @@
         <v>80</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1104,10 +1104,10 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1115,10 +1115,10 @@
         <v>82</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1126,10 +1126,10 @@
         <v>83</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1137,10 +1137,10 @@
         <v>84</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1161,7 +1161,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>106</v>
@@ -1169,7 +1169,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>107</v>
@@ -1258,7 +1258,7 @@
         <v>94</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1272,7 +1272,7 @@
         <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1280,7 +1280,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1288,7 +1288,7 @@
         <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1296,7 +1296,7 @@
         <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1304,7 +1304,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1312,7 +1312,7 @@
         <v>35</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1344,7 +1344,7 @@
         <v>39</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1352,7 +1352,7 @@
         <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1368,7 +1368,7 @@
         <v>42</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1376,7 +1376,7 @@
         <v>43</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1384,7 +1384,7 @@
         <v>44</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1392,7 +1392,7 @@
         <v>45</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1400,7 +1400,7 @@
         <v>46</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1408,7 +1408,7 @@
         <v>47</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1416,7 +1416,7 @@
         <v>48</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1424,7 +1424,7 @@
         <v>49</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1432,7 +1432,7 @@
         <v>50</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1440,7 +1440,7 @@
         <v>51</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1448,7 +1448,7 @@
         <v>52</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1456,7 +1456,7 @@
         <v>53</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1464,7 +1464,7 @@
         <v>54</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1472,7 +1472,7 @@
         <v>55</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:4">

</xml_diff>

<commit_message>
Updated with api html and build candidate resume method implementation
</commit_message>
<xml_diff>
--- a/docs/JB.xlsx
+++ b/docs/JB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="141">
   <si>
     <t>US ID</t>
   </si>
@@ -443,6 +443,15 @@
   </si>
   <si>
     <t>As an Employer I am able to maintain the view count while viewing the resumes(resumeId)</t>
+  </si>
+  <si>
+    <t>JB_US_33</t>
+  </si>
+  <si>
+    <t>As a Candidate I am able to build the resume</t>
+  </si>
+  <si>
+    <t>/api/resume/build/candidate</t>
   </si>
 </sst>
 </file>
@@ -805,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -884,10 +893,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>62</v>
+        <v>139</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -895,10 +904,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -906,10 +915,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -917,10 +926,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -928,10 +937,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -939,10 +948,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -950,10 +959,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -961,10 +970,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -972,10 +981,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -983,10 +992,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -994,10 +1003,10 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1005,10 +1014,10 @@
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1016,10 +1025,10 @@
         <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1027,10 +1036,10 @@
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1038,10 +1047,10 @@
         <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1049,10 +1058,10 @@
         <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>137</v>
+        <v>76</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1060,10 +1069,10 @@
         <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1071,10 +1080,10 @@
         <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1082,10 +1091,10 @@
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1093,10 +1102,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1104,10 +1113,10 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1115,10 +1124,10 @@
         <v>82</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1126,10 +1135,10 @@
         <v>83</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1137,10 +1146,10 @@
         <v>84</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1148,7 +1157,10 @@
         <v>85</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1156,7 +1168,7 @@
         <v>86</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1164,7 +1176,7 @@
         <v>116</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1172,6 +1184,14 @@
         <v>117</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>